<commit_message>
hw: update resistors R20-R23 value in parts_SMT.xlsx
</commit_message>
<xml_diff>
--- a/hw/parts_SMT.xlsx
+++ b/hw/parts_SMT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sandbox\_Track\RB3204-RBCX\hw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4A2E37-4E68-406A-8931-A0D847A15B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18720" windowHeight="7860"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import from Eagle BOM" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Import from Eagle BOM'!$A$1:$X$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="274">
   <si>
     <t>Description</t>
   </si>
@@ -217,9 +228,6 @@
     <t>0402CG180J500NT</t>
   </si>
   <si>
-    <t>R16, R17, R18, R19, R20, R21, R22, R23, R81, R82, R117, R118, R139, R141, R143, R145</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -289,9 +297,6 @@
     <t>0402WGF2402TCE</t>
   </si>
   <si>
-    <t>R14, R15, R120, R121, R122, R123, R127, R128, R129, R130, R147, R148, R149, R150, R151</t>
-  </si>
-  <si>
     <t>2k2</t>
   </si>
   <si>
@@ -842,12 +847,21 @@
   </si>
   <si>
     <t>Price if 1 PCB</t>
+  </si>
+  <si>
+    <t>R16, R17, R18, R19, R81, R82, R117, R118, R139, R141, R143, R145</t>
+  </si>
+  <si>
+    <t>R14, R15,R20, R21, R22, R23,  R120, R121, R122, R123, R127, R128, R129, R130, R147, R148, R149, R150, R151</t>
+  </si>
+  <si>
+    <t>R14, R15, R20, R21, R22, R23, R120, R121, R122, R123, R127, R128, R129, R130, R147, R148, R149, R150, R151</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
@@ -1030,7 +1044,7 @@
     <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1059,7 +1073,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Export for JLCPCB-style" pivot="0" count="3">
+    <tableStyle name="Export for JLCPCB-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -1077,14 +1091,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:F39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:F39">
   <tableColumns count="6">
-    <tableColumn id="1" name="Qty"/>
-    <tableColumn id="2" name="Designator"/>
-    <tableColumn id="3" name="Footprint"/>
-    <tableColumn id="4" name="Comment"/>
-    <tableColumn id="5" name="LCSC Part # (optional)"/>
-    <tableColumn id="6" name="Description (optional)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Designator"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Footprint"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Comment"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LCSC Part # (optional)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description (optional)"/>
   </tableColumns>
   <tableStyleInfo name="Export for JLCPCB-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1287,14 +1301,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="T7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA6" sqref="AA6"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1394,57 +1408,57 @@
         <v>57</v>
       </c>
       <c r="X1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="14" t="s">
-        <v>70</v>
-      </c>
       <c r="Z1" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA1" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB1" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AC1" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B2" s="16">
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>191</v>
-      </c>
       <c r="F2" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J2" s="18">
         <v>100</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L2" s="20">
         <v>2.4287000000000001</v>
@@ -1479,7 +1493,7 @@
       <c r="V2" s="17"/>
       <c r="W2" s="38"/>
       <c r="X2" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Y2" s="24">
         <f>B2*L2+ (B2*J2*0.0015)</f>
@@ -1500,44 +1514,44 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B3" s="26">
         <v>1</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>175</v>
-      </c>
       <c r="F3" s="35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J3" s="35">
         <v>24</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L3" s="31">
         <v>2.1715</v>
       </c>
       <c r="M3" s="26"/>
       <c r="N3" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P3" s="26"/>
       <c r="Q3" s="26"/>
@@ -1550,7 +1564,7 @@
       <c r="V3" s="26"/>
       <c r="W3" s="26"/>
       <c r="X3" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Y3" s="24">
         <f t="shared" ref="Y3:Y39" si="1">B3*L3+ (B3*J3*0.0015)</f>
@@ -1579,31 +1593,31 @@
         <v>2</v>
       </c>
       <c r="C4" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>163</v>
-      </c>
       <c r="G4" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J4" s="29">
         <v>16</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L4" s="41">
         <v>0.51549999999999996</v>
@@ -1624,7 +1638,7 @@
       <c r="V4" s="28"/>
       <c r="W4" s="39"/>
       <c r="X4" s="28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Y4" s="24">
         <f t="shared" si="1"/>
@@ -1649,44 +1663,44 @@
         <v>2</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D5" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>179</v>
-      </c>
       <c r="F5" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J5" s="26">
         <v>8</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L5" s="31">
         <v>0.4798</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N5" s="35" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O5" s="26"/>
       <c r="P5" s="35" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Q5" s="26"/>
       <c r="R5" s="35"/>
@@ -1698,7 +1712,7 @@
       <c r="V5" s="26"/>
       <c r="W5" s="26"/>
       <c r="X5" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Y5" s="24">
         <f t="shared" si="1"/>
@@ -1723,31 +1737,31 @@
         <v>8</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J6" s="18">
         <v>5</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L6" s="36">
         <v>0.39429999999999998</v>
@@ -1778,7 +1792,7 @@
       <c r="V6" s="17"/>
       <c r="W6" s="38"/>
       <c r="X6" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Y6" s="24">
         <f t="shared" si="1"/>
@@ -1803,37 +1817,37 @@
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B7" s="16">
         <v>1</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>124</v>
-      </c>
       <c r="G7" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J7" s="18">
         <v>2</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L7" s="36">
         <v>0.17069999999999999</v>
@@ -1854,7 +1868,7 @@
       <c r="V7" s="17"/>
       <c r="W7" s="38"/>
       <c r="X7" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Y7" s="24">
         <f t="shared" si="1"/>
@@ -1875,37 +1889,37 @@
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B8" s="26">
         <v>1</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D8" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="F8" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>268</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>110</v>
-      </c>
       <c r="I8" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J8" s="29">
         <v>2</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L8" s="41">
         <v>0.1542</v>
@@ -1926,7 +1940,7 @@
       <c r="V8" s="28"/>
       <c r="W8" s="39"/>
       <c r="X8" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Y8" s="24">
         <f t="shared" si="1"/>
@@ -1947,37 +1961,37 @@
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B9" s="16">
         <v>1</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D9" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>139</v>
-      </c>
       <c r="F9" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J9" s="18">
         <v>4</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L9" s="36">
         <v>0.123</v>
@@ -2000,7 +2014,7 @@
       </c>
       <c r="W9" s="38"/>
       <c r="X9" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Y9" s="24">
         <f t="shared" si="1"/>
@@ -2021,28 +2035,28 @@
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B10" s="26">
         <v>8</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D10" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>129</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>131</v>
       </c>
       <c r="I10" s="28" t="s">
         <v>26</v>
@@ -2051,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L10" s="41">
         <v>7.9399999999999998E-2</v>
@@ -2072,7 +2086,7 @@
       <c r="V10" s="28"/>
       <c r="W10" s="28"/>
       <c r="X10" s="28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Y10" s="24">
         <f t="shared" si="1"/>
@@ -2097,37 +2111,37 @@
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B11" s="16">
         <v>2</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>166</v>
-      </c>
       <c r="I11" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J11" s="18">
         <v>2</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L11" s="36">
         <v>4.07E-2</v>
@@ -2148,7 +2162,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="38"/>
       <c r="X11" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="Y11" s="24">
         <f t="shared" si="1"/>
@@ -2173,31 +2187,31 @@
         <v>4</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D12" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="26" t="s">
-        <v>144</v>
-      </c>
       <c r="F12" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J12" s="29">
         <v>2</v>
       </c>
       <c r="K12" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L12" s="41">
         <v>3.4200000000000001E-2</v>
@@ -2218,7 +2232,7 @@
       <c r="V12" s="28"/>
       <c r="W12" s="39"/>
       <c r="X12" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Y12" s="24">
         <f t="shared" si="1"/>
@@ -2239,37 +2253,37 @@
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B13" s="26">
         <v>13</v>
       </c>
       <c r="C13" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="G13" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>148</v>
-      </c>
       <c r="I13" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J13" s="29">
         <v>3</v>
       </c>
       <c r="K13" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L13" s="31">
         <v>3.3799999999999997E-2</v>
@@ -2290,7 +2304,7 @@
       <c r="V13" s="28"/>
       <c r="W13" s="39"/>
       <c r="X13" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Y13" s="24">
         <f t="shared" si="1"/>
@@ -2315,31 +2329,31 @@
         <v>12</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D14" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>187</v>
-      </c>
       <c r="F14" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J14" s="18">
         <v>2</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L14" s="20">
         <v>3.3500000000000002E-2</v>
@@ -2360,7 +2374,7 @@
       <c r="V14" s="17"/>
       <c r="W14" s="38"/>
       <c r="X14" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Y14" s="24">
         <f t="shared" si="1"/>
@@ -2381,37 +2395,37 @@
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B15" s="16">
         <v>2</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D15" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="I15" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J15" s="18">
         <v>3</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L15" s="36">
         <v>2.93E-2</v>
@@ -2432,7 +2446,7 @@
       <c r="V15" s="17"/>
       <c r="W15" s="38"/>
       <c r="X15" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Y15" s="24">
         <f t="shared" si="1"/>
@@ -2453,37 +2467,37 @@
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B16" s="16">
         <v>2</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D16" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>155</v>
-      </c>
       <c r="F16" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J16" s="18">
         <v>2</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L16" s="20">
         <v>2.6700000000000002E-2</v>
@@ -2504,7 +2518,7 @@
       <c r="V16" s="17"/>
       <c r="W16" s="38"/>
       <c r="X16" s="17" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Y16" s="24">
         <f t="shared" si="1"/>
@@ -2525,37 +2539,37 @@
     </row>
     <row r="17" spans="1:28">
       <c r="A17" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B17" s="26">
         <v>2</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D17" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="E17" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="H17" s="28" t="s">
-        <v>195</v>
-      </c>
       <c r="I17" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J17" s="29">
         <v>2</v>
       </c>
       <c r="K17" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L17" s="31">
         <v>2.6200000000000001E-2</v>
@@ -2576,7 +2590,7 @@
       <c r="V17" s="28"/>
       <c r="W17" s="39"/>
       <c r="X17" s="28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Y17" s="24">
         <f t="shared" si="1"/>
@@ -2597,13 +2611,13 @@
     </row>
     <row r="18" spans="1:28">
       <c r="A18" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B18" s="16">
         <v>13</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>54</v>
@@ -2615,7 +2629,7 @@
         <v>59</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>58</v>
@@ -2627,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L18" s="20">
         <v>2.2100000000000002E-2</v>
@@ -2649,10 +2663,10 @@
         <v>25</v>
       </c>
       <c r="W18" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X18" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y18" s="24">
         <f t="shared" si="1"/>
@@ -2677,31 +2691,31 @@
         <v>8</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D19" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>99</v>
-      </c>
       <c r="F19" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J19" s="18">
         <v>3</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L19" s="36">
         <v>2.18E-2</v>
@@ -2722,7 +2736,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="38"/>
       <c r="X19" s="17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Y19" s="24">
         <f t="shared" si="1"/>
@@ -2743,37 +2757,37 @@
     </row>
     <row r="20" spans="1:28">
       <c r="A20" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" s="26">
         <v>3</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D20" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="F20" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>105</v>
-      </c>
       <c r="G20" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J20" s="29">
         <v>2</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L20" s="41">
         <v>1.03E-2</v>
@@ -2795,10 +2809,10 @@
         <v>16</v>
       </c>
       <c r="W20" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X20" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y20" s="24">
         <f t="shared" si="1"/>
@@ -2819,13 +2833,13 @@
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B21" s="16">
         <v>3</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>48</v>
@@ -2837,7 +2851,7 @@
         <v>52</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>51</v>
@@ -2849,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L21" s="36">
         <v>8.3000000000000001E-3</v>
@@ -2871,10 +2885,10 @@
         <v>50</v>
       </c>
       <c r="W21" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X21" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y21" s="24">
         <f t="shared" si="1"/>
@@ -2895,13 +2909,13 @@
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B22" s="16">
         <v>5</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>24</v>
@@ -2913,7 +2927,7 @@
         <v>31</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>29</v>
@@ -2925,7 +2939,7 @@
         <v>2</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L22" s="20">
         <v>8.2000000000000007E-3</v>
@@ -2946,7 +2960,7 @@
       <c r="V22" s="17"/>
       <c r="W22" s="17"/>
       <c r="X22" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Y22" s="24">
         <f t="shared" si="1"/>
@@ -2967,37 +2981,37 @@
     </row>
     <row r="23" spans="1:28" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B23" s="26">
         <v>18</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D23" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="H23" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="E23" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>183</v>
-      </c>
       <c r="I23" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J23" s="29">
         <v>2</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L23" s="41">
         <v>7.9000000000000008E-3</v>
@@ -3018,7 +3032,7 @@
       <c r="V23" s="28"/>
       <c r="W23" s="39"/>
       <c r="X23" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Y23" s="24">
         <f t="shared" si="1"/>
@@ -3039,28 +3053,28 @@
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B24" s="16">
         <v>10</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>39</v>
@@ -3069,7 +3083,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L24" s="20">
         <v>7.7999999999999996E-3</v>
@@ -3091,10 +3105,10 @@
         <v>25</v>
       </c>
       <c r="W24" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X24" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y24" s="24">
         <f t="shared" si="1"/>
@@ -3115,13 +3129,13 @@
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B25" s="26">
         <v>16</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>38</v>
@@ -3133,7 +3147,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H25" s="28" t="s">
         <v>42</v>
@@ -3145,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L25" s="31">
         <v>4.3E-3</v>
@@ -3167,10 +3181,10 @@
         <v>16</v>
       </c>
       <c r="W25" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X25" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y25" s="24">
         <f t="shared" si="1"/>
@@ -3191,13 +3205,13 @@
     </row>
     <row r="26" spans="1:28" ht="15.75" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" s="16">
         <v>2</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>60</v>
@@ -3209,7 +3223,7 @@
         <v>63</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>62</v>
@@ -3221,7 +3235,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L26" s="20">
         <v>1.9E-3</v>
@@ -3243,10 +3257,10 @@
         <v>50</v>
       </c>
       <c r="W26" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="X26" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y26" s="24">
         <f t="shared" si="1"/>
@@ -3267,13 +3281,13 @@
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1">
       <c r="A27" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B27" s="26">
         <v>6</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>32</v>
@@ -3285,7 +3299,7 @@
         <v>37</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>36</v>
@@ -3297,7 +3311,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L27" s="31">
         <v>1.9E-3</v>
@@ -3318,7 +3332,7 @@
       <c r="V27" s="28"/>
       <c r="W27" s="28"/>
       <c r="X27" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y27" s="24">
         <f t="shared" si="1"/>
@@ -3339,28 +3353,28 @@
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B28" s="26">
         <v>1</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D28" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="F28" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="35" t="s">
-        <v>96</v>
-      </c>
       <c r="G28" s="35" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H28" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I28" s="26" t="s">
         <v>39</v>
@@ -3369,7 +3383,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L28" s="41">
         <v>1.8E-3</v>
@@ -3380,18 +3394,18 @@
       <c r="Q28" s="26"/>
       <c r="R28" s="26"/>
       <c r="S28" s="35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="T28" s="26"/>
       <c r="U28" s="34">
         <v>43960</v>
       </c>
       <c r="V28" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="W28" s="26"/>
       <c r="X28" s="35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Y28" s="24">
         <f t="shared" si="1"/>
@@ -3412,28 +3426,28 @@
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1">
       <c r="A29" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B29" s="26">
         <v>2</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D29" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="H29" s="28" t="s">
         <v>133</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="H29" s="28" t="s">
-        <v>135</v>
       </c>
       <c r="I29" s="28" t="s">
         <v>39</v>
@@ -3442,7 +3456,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L29" s="31">
         <v>1.8E-3</v>
@@ -3464,10 +3478,10 @@
         <v>50</v>
       </c>
       <c r="W29" s="33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="X29" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Y29" s="24">
         <f t="shared" si="1"/>
@@ -3488,13 +3502,13 @@
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B30" s="26">
         <v>7</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>17</v>
@@ -3506,7 +3520,7 @@
         <v>21</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H30" s="26" t="s">
         <v>20</v>
@@ -3518,7 +3532,7 @@
         <v>2</v>
       </c>
       <c r="K30" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L30" s="41">
         <v>1.6000000000000001E-3</v>
@@ -3530,7 +3544,7 @@
       <c r="Q30" s="26"/>
       <c r="R30" s="26"/>
       <c r="S30" s="35" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="T30" s="35"/>
       <c r="U30" s="34">
@@ -3539,7 +3553,7 @@
       <c r="V30" s="26"/>
       <c r="W30" s="26"/>
       <c r="X30" s="35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="Y30" s="24">
         <f t="shared" si="1"/>
@@ -3560,28 +3574,28 @@
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1">
       <c r="A31" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B31" s="16">
         <v>2</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="H31" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>86</v>
       </c>
       <c r="I31" s="17" t="s">
         <v>34</v>
@@ -3590,7 +3604,7 @@
         <v>2</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L31" s="36">
         <v>1.1000000000000001E-3</v>
@@ -3611,7 +3625,7 @@
       <c r="V31" s="17"/>
       <c r="W31" s="17"/>
       <c r="X31" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y31" s="24">
         <f t="shared" si="1"/>
@@ -3632,28 +3646,28 @@
     </row>
     <row r="32" spans="1:28" ht="15.75" customHeight="1">
       <c r="A32" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B32" s="26">
         <v>2</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D32" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="H32" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="H32" s="28" t="s">
-        <v>127</v>
       </c>
       <c r="I32" s="28" t="s">
         <v>34</v>
@@ -3662,7 +3676,7 @@
         <v>2</v>
       </c>
       <c r="K32" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L32" s="41">
         <v>1.1000000000000001E-3</v>
@@ -3683,7 +3697,7 @@
       <c r="V32" s="28"/>
       <c r="W32" s="28"/>
       <c r="X32" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y32" s="24">
         <f t="shared" si="1"/>
@@ -3704,28 +3718,28 @@
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1">
       <c r="A33" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B33" s="16">
         <v>17</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D33" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="H33" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>118</v>
       </c>
       <c r="I33" s="17" t="s">
         <v>34</v>
@@ -3734,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L33" s="36">
         <v>8.9999999999999998E-4</v>
@@ -3755,7 +3769,7 @@
       <c r="V33" s="17"/>
       <c r="W33" s="17"/>
       <c r="X33" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y33" s="24">
         <f t="shared" si="1"/>
@@ -3776,28 +3790,28 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1">
       <c r="A34" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B34" s="16">
+        <v>19</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="B34" s="16">
-        <v>15</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="H34" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>34</v>
@@ -3806,7 +3820,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L34" s="20">
         <v>8.9999999999999998E-4</v>
@@ -3827,15 +3841,15 @@
       <c r="V34" s="17"/>
       <c r="W34" s="17"/>
       <c r="X34" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y34" s="24">
         <f t="shared" si="1"/>
-        <v>5.8499999999999996E-2</v>
+        <v>7.4099999999999999E-2</v>
       </c>
       <c r="Z34" s="25">
         <f t="shared" si="2"/>
-        <v>750</v>
+        <v>950</v>
       </c>
       <c r="AA34" s="24">
         <f t="shared" si="0"/>
@@ -3843,33 +3857,33 @@
       </c>
       <c r="AB34" s="44">
         <f t="shared" si="3"/>
-        <v>5.8499999999999996E-2</v>
+        <v>7.4099999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1">
       <c r="A35" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="B35" s="26">
+        <v>12</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="B35" s="26">
-        <v>16</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="26" t="s">
+      <c r="H35" s="28" t="s">
         <v>65</v>
-      </c>
-      <c r="F35" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="H35" s="28" t="s">
-        <v>66</v>
       </c>
       <c r="I35" s="28" t="s">
         <v>34</v>
@@ -3878,7 +3892,7 @@
         <v>2</v>
       </c>
       <c r="K35" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L35" s="31">
         <v>8.9999999999999998E-4</v>
@@ -3899,15 +3913,15 @@
       <c r="V35" s="28"/>
       <c r="W35" s="28"/>
       <c r="X35" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y35" s="24">
         <f t="shared" si="1"/>
-        <v>6.2399999999999997E-2</v>
+        <v>4.6800000000000008E-2</v>
       </c>
       <c r="Z35" s="25">
         <f t="shared" si="2"/>
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="AA35" s="24">
         <f t="shared" si="0"/>
@@ -3915,18 +3929,18 @@
       </c>
       <c r="AB35" s="44">
         <f t="shared" si="3"/>
-        <v>6.2399999999999997E-2</v>
+        <v>4.6800000000000008E-2</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="15.75" customHeight="1">
       <c r="A36" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B36" s="16">
         <v>8</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>44</v>
@@ -3938,7 +3952,7 @@
         <v>47</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>46</v>
@@ -3950,7 +3964,7 @@
         <v>2</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L36" s="20">
         <v>8.9999999999999998E-4</v>
@@ -3971,7 +3985,7 @@
       <c r="V36" s="17"/>
       <c r="W36" s="17"/>
       <c r="X36" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y36" s="24">
         <f t="shared" si="1"/>
@@ -3992,28 +4006,28 @@
     </row>
     <row r="37" spans="1:29" ht="15.75" customHeight="1">
       <c r="A37" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B37" s="26">
         <v>76</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D37" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="H37" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="H37" s="28" t="s">
-        <v>114</v>
       </c>
       <c r="I37" s="28" t="s">
         <v>34</v>
@@ -4022,7 +4036,7 @@
         <v>2</v>
       </c>
       <c r="K37" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L37" s="31">
         <v>8.9999999999999998E-4</v>
@@ -4043,7 +4057,7 @@
       <c r="V37" s="28"/>
       <c r="W37" s="28"/>
       <c r="X37" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y37" s="24">
         <f t="shared" si="1"/>
@@ -4064,28 +4078,28 @@
     </row>
     <row r="38" spans="1:29" ht="15.75" customHeight="1">
       <c r="A38" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B38" s="26">
         <v>1</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D38" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="F38" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="H38" s="28" t="s">
         <v>75</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="G38" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="H38" s="28" t="s">
-        <v>76</v>
       </c>
       <c r="I38" s="28" t="s">
         <v>34</v>
@@ -4094,7 +4108,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L38" s="41">
         <v>8.9999999999999998E-4</v>
@@ -4115,7 +4129,7 @@
       <c r="V38" s="28"/>
       <c r="W38" s="28"/>
       <c r="X38" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y38" s="24">
         <f t="shared" si="1"/>
@@ -4136,37 +4150,37 @@
     </row>
     <row r="39" spans="1:29" ht="15.75" customHeight="1">
       <c r="A39" s="16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B39" s="16">
         <v>1</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="H39" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="I39" s="17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J39" s="18">
         <v>2</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L39" s="36">
         <v>8.9999999999999998E-4</v>
@@ -4187,7 +4201,7 @@
       <c r="V39" s="17"/>
       <c r="W39" s="17"/>
       <c r="X39" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y39" s="24">
         <f t="shared" si="1"/>
@@ -4233,7 +4247,7 @@
       <c r="X40" s="17"/>
       <c r="Y40" s="24">
         <f>SUM(Y2:Y39)</f>
-        <v>14.2521</v>
+        <v>14.252099999999999</v>
       </c>
       <c r="Z40" s="18"/>
       <c r="AA40" s="44">
@@ -4242,7 +4256,7 @@
       </c>
       <c r="AB40" s="44">
         <f>SUM(AB2:AB39)*5</f>
-        <v>71.260500000000008</v>
+        <v>71.260499999999993</v>
       </c>
       <c r="AC40">
         <f>SUM(AC2:AC39)</f>
@@ -7132,8 +7146,8 @@
       <c r="L1000" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X39">
-    <sortState ref="A2:X40">
+  <autoFilter ref="A1:X39" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X40">
       <sortCondition descending="1" ref="L1:L39"/>
     </sortState>
   </autoFilter>
@@ -7143,13 +7157,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7343,22 +7359,22 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>271</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -7366,19 +7382,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7386,19 +7402,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -7406,19 +7422,19 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -7426,39 +7442,39 @@
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>88</v>
+        <v>273</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7466,19 +7482,19 @@
         <v>1</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -7486,19 +7502,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="F17" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7506,19 +7522,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="F18" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -7526,19 +7542,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="15" t="s">
+      <c r="E19" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="F19" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -7546,19 +7562,19 @@
         <v>76</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -7566,19 +7582,19 @@
         <v>17</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -7586,19 +7602,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="F22" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -7606,19 +7622,19 @@
         <v>2</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -7626,19 +7642,19 @@
         <v>8</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -7646,19 +7662,19 @@
         <v>2</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -7666,19 +7682,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="F26" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7686,19 +7702,19 @@
         <v>4</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="F27" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7706,19 +7722,19 @@
         <v>13</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="F28" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7726,19 +7742,19 @@
         <v>2</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="F29" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -7746,19 +7762,19 @@
         <v>2</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -7766,19 +7782,19 @@
         <v>2</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="F31" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -7786,19 +7802,19 @@
         <v>2</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="F32" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -7806,19 +7822,19 @@
         <v>8</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="F33" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -7826,19 +7842,19 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>176</v>
-      </c>
       <c r="F34" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -7846,19 +7862,19 @@
         <v>2</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="E35" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="F35" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -7866,19 +7882,19 @@
         <v>18</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="F36" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -7886,19 +7902,19 @@
         <v>12</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>188</v>
-      </c>
       <c r="F37" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -7906,19 +7922,19 @@
         <v>1</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>192</v>
-      </c>
       <c r="F38" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -7926,19 +7942,19 @@
         <v>2</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="F39" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>